<commit_message>
feat: add dashboard charts to DASHBOARD_TRENDS tab (#163)
Three charts added to the workbook via openpyxl:
- Line chart: ActiveDecisions + AvgConfidence over time
- Bar chart: OpenPatches + REDPatches by week (RED in red)
- Area chart: AvgPromptHealth trend

All charts reference DashboardTrendsTable columns and auto-update
when new trend rows are added.

Closes #163

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/artifacts/excel/Coherence_Prompt_OS_v2.xlsx
+++ b/artifacts/excel/Coherence_Prompt_OS_v2.xlsx
@@ -151,6 +151,482 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Decisions &amp; Confidence Trend</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'DASHBOARD_TRENDS'!B1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25000">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'DASHBOARD_TRENDS'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'DASHBOARD_TRENDS'!$B$2:$B$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'DASHBOARD_TRENDS'!C1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25000">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'DASHBOARD_TRENDS'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'DASHBOARD_TRENDS'!$C$2:$C$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Week</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Value</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Patches by Week</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'DASHBOARD_TRENDS'!F1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'DASHBOARD_TRENDS'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'DASHBOARD_TRENDS'!$F$2:$F$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'DASHBOARD_TRENDS'!G1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'DASHBOARD_TRENDS'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'DASHBOARD_TRENDS'!$G$2:$G$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Week</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Count</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Prompt Health Trend</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <areaChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'DASHBOARD_TRENDS'!H1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="4472C4"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'DASHBOARD_TRENDS'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'DASHBOARD_TRENDS'!$H$2:$H$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </areaChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Week</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Health (0–100)</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>6</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="7200000" cy="4320000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>22</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="7200000" cy="4320000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>38</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="7200000" cy="4320000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="3" name="Chart 3"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2276,8 +2752,6 @@
           <t>2026-02-10</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
           <t>Monitor HR announcements</t>
@@ -2325,8 +2799,6 @@
           <t>2026-02-12</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
           <t>Escalated to architecture review</t>
@@ -2374,7 +2846,6 @@
           <t>2026-02-15</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
           <t>Scheduling v2 parity test</t>
@@ -2652,7 +3123,6 @@
         <f>COUNTIF(DecisionLogTable[Status],"Active")</f>
         <v/>
       </c>
-      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
           <t>2026-02-18</t>
@@ -2669,7 +3139,6 @@
         <f>AVERAGE(DecisionLogTable[Confidence_pct])</f>
         <v/>
       </c>
-      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
           <t>2026-02-18</t>
@@ -2686,7 +3155,6 @@
         <f>COUNTIF(AtomicClaimsTable[CredibilityScore],"&lt;60")</f>
         <v/>
       </c>
-      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
           <t>2026-02-18</t>
@@ -2703,7 +3171,6 @@
         <f>COUNTIF(AssumptionsTable[ExpiryRisk],"RED")</f>
         <v/>
       </c>
-      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
           <t>2026-02-18</t>
@@ -2720,7 +3187,6 @@
         <f>COUNTIF(PatchLogTable[Status],"Open")</f>
         <v/>
       </c>
-      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
           <t>2026-02-18</t>
@@ -2737,7 +3203,6 @@
         <f>COUNTIF(PatchLogTable[Severity_GYR],"RED")</f>
         <v/>
       </c>
-      <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
           <t>2026-02-18</t>
@@ -2754,7 +3219,6 @@
         <f>AVERAGE(PromptLibraryTable[PromptHealth])</f>
         <v/>
       </c>
-      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
           <t>2026-02-18</t>
@@ -2771,7 +3235,6 @@
         <f>COUNTIF(PromptLibraryTable[DriftFlag],"Major")</f>
         <v/>
       </c>
-      <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
           <t>2026-02-18</t>
@@ -2784,8 +3247,6 @@
           <t>Last LLM Run Confidence</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
           <t>2026-02-18</t>
@@ -2802,7 +3263,6 @@
         <f>COUNTA(LLMOutputTable[RunID])</f>
         <v/>
       </c>
-      <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
           <t>2026-02-18</t>
@@ -2987,8 +3447,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
feat: add sealed run exporter + workbook enum dropdowns
New scripts/prompt_os/export_sealed_run.py exports a single RunID from
llm_output.csv to an immutable JSON snapshot in artifacts/sealed_runs/.
Also adds data validation dropdowns to the workbook for all enum columns
across 5 tabs (12 dropdowns total).

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/artifacts/excel/Coherence_Prompt_OS_v2.xlsx
+++ b/artifacts/excel/Coherence_Prompt_OS_v2.xlsx
@@ -155,7 +155,6 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="10"/>
   <chart>
     <title>
       <tx>
@@ -306,7 +305,6 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="10"/>
   <chart>
     <title>
       <tx>
@@ -446,7 +444,6 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="10"/>
   <chart>
     <title>
       <tx>
@@ -502,21 +499,6 @@
           <orientation val="minMax"/>
         </scaling>
         <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Week</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
         <crossAx val="100"/>
@@ -529,21 +511,6 @@
         </scaling>
         <axPos val="l"/>
         <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Health (0–100)</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
         <crossAx val="10"/>
@@ -1421,6 +1388,20 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="4">
+    <dataValidation sqref="C2:C1000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Use the dropdown." promptTitle="Allowed Values" prompt="Select from list" type="list">
+      <formula1>"Technology,Operations,Finance,Strategy,People"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Use the dropdown." promptTitle="Allowed Values" prompt="Select from list" type="list">
+      <formula1>"Active,Deferred,Closed,Superseded"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I2:I1000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Use the dropdown." promptTitle="Allowed Values" prompt="Select from list" type="list">
+      <formula1>"Low,Medium,High"</formula1>
+    </dataValidation>
+    <dataValidation sqref="J2:J1000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Use the dropdown." promptTitle="Allowed Values" prompt="Select from list" type="list">
+      <formula1>"Low,Medium,High"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
@@ -1980,6 +1961,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="D2:D1000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Use the dropdown." promptTitle="Allowed Values" prompt="Select from list" type="list">
+      <formula1>"Internal,External,LLM,Expert"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
@@ -2298,6 +2284,14 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="C2:C1000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Use the dropdown." promptTitle="Allowed Values" prompt="Select from list" type="list">
+      <formula1>"Decision,Perception,Governance,Maintenance,Analysis"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Use the dropdown." promptTitle="Allowed Values" prompt="Select from list" type="list">
+      <formula1>"None,Minor,Major"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
@@ -2620,6 +2614,14 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="H2:H1000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Use the dropdown." promptTitle="Allowed Values" prompt="Select from list" type="list">
+      <formula1>"RED,YELLOW,GREEN"</formula1>
+    </dataValidation>
+    <dataValidation sqref="K2:K1000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Use the dropdown." promptTitle="Allowed Values" prompt="Select from list" type="list">
+      <formula1>"Active,Expired,Validated,Invalidated"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
@@ -2858,6 +2860,17 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation sqref="B2:B1000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Use the dropdown." promptTitle="Allowed Values" prompt="Select from list" type="list">
+      <formula1>"Drift,Expiry,Manual,LLM"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Use the dropdown." promptTitle="Allowed Values" prompt="Select from list" type="list">
+      <formula1>"GREEN,YELLOW,RED"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1000" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Use the dropdown." promptTitle="Allowed Values" prompt="Select from list" type="list">
+      <formula1>"Open,In Progress,Resolved,Wont Fix"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>